<commit_message>
Response XML size statistics updated
</commit_message>
<xml_diff>
--- a/documentation/src/main/resources/Response sizes.xlsx
+++ b/documentation/src/main/resources/Response sizes.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -381,10 +381,10 @@
         <v>1000</v>
       </c>
       <c r="B2">
-        <v>655</v>
+        <v>609</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -392,10 +392,10 @@
         <v>2000</v>
       </c>
       <c r="B3">
-        <v>1122</v>
+        <v>1013</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -403,10 +403,10 @@
         <v>3000</v>
       </c>
       <c r="B4">
-        <v>1610</v>
+        <v>1510</v>
       </c>
       <c r="C4">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -414,10 +414,10 @@
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>2153</v>
+        <v>2022</v>
       </c>
       <c r="C5">
-        <v>176</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -425,10 +425,10 @@
         <v>5000</v>
       </c>
       <c r="B6">
-        <v>2676</v>
+        <v>2514</v>
       </c>
       <c r="C6">
-        <v>220</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -436,10 +436,10 @@
         <v>6000</v>
       </c>
       <c r="B7">
-        <v>3263</v>
+        <v>3057</v>
       </c>
       <c r="C7">
-        <v>264</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -447,10 +447,10 @@
         <v>7000</v>
       </c>
       <c r="B8">
-        <v>3735</v>
+        <v>3507</v>
       </c>
       <c r="C8">
-        <v>308</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -458,10 +458,10 @@
         <v>8000</v>
       </c>
       <c r="B9">
-        <v>4275</v>
+        <v>4013</v>
       </c>
       <c r="C9">
-        <v>353</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -469,10 +469,10 @@
         <v>9000</v>
       </c>
       <c r="B10">
-        <v>4847</v>
+        <v>4591</v>
       </c>
       <c r="C10">
-        <v>397</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -480,10 +480,10 @@
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>5485</v>
+        <v>5038</v>
       </c>
       <c r="C11">
-        <v>441</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -491,10 +491,10 @@
         <v>11000</v>
       </c>
       <c r="B12">
-        <v>5992</v>
+        <v>5740</v>
       </c>
       <c r="C12">
-        <v>485</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -502,10 +502,10 @@
         <v>12000</v>
       </c>
       <c r="B13">
-        <v>6633</v>
+        <v>6073</v>
       </c>
       <c r="C13">
-        <v>529</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -513,10 +513,10 @@
         <v>13000</v>
       </c>
       <c r="B14">
-        <v>7205</v>
+        <v>6680</v>
       </c>
       <c r="C14">
-        <v>573</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -524,10 +524,10 @@
         <v>14000</v>
       </c>
       <c r="B15">
-        <v>7638</v>
+        <v>7361</v>
       </c>
       <c r="C15">
-        <v>617</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -535,10 +535,10 @@
         <v>15000</v>
       </c>
       <c r="B16">
-        <v>8125</v>
+        <v>7727</v>
       </c>
       <c r="C16">
-        <v>661</v>
+        <v>547</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -546,10 +546,10 @@
         <v>16000</v>
       </c>
       <c r="B17">
-        <v>8721</v>
+        <v>8203</v>
       </c>
       <c r="C17">
-        <v>706</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -557,10 +557,10 @@
         <v>17000</v>
       </c>
       <c r="B18">
-        <v>9200</v>
+        <v>8986</v>
       </c>
       <c r="C18">
-        <v>750</v>
+        <v>620</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -568,10 +568,10 @@
         <v>18000</v>
       </c>
       <c r="B19">
-        <v>9754</v>
+        <v>9519</v>
       </c>
       <c r="C19">
-        <v>794</v>
+        <v>657</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -579,10 +579,10 @@
         <v>19000</v>
       </c>
       <c r="B20">
-        <v>10184</v>
+        <v>9685</v>
       </c>
       <c r="C20">
-        <v>838</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -590,10 +590,10 @@
         <v>20000</v>
       </c>
       <c r="B21">
-        <v>10795</v>
+        <v>10230</v>
       </c>
       <c r="C21">
-        <v>882</v>
+        <v>729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>